<commit_message>
few improvement related to header and cleaning
</commit_message>
<xml_diff>
--- a/out/RMRP_2021_AI_consolidated.xlsx
+++ b/out/RMRP_2021_AI_consolidated.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M29"/>
+  <dimension ref="A1:M40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -436,16 +436,16 @@
         </is>
       </c>
       <c r="C2">
-        <v>27</v>
+        <v>3266</v>
       </c>
       <c r="D2">
-        <v>27</v>
+        <v>2777</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>489</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -454,16 +454,19 @@
         <v>0</v>
       </c>
       <c r="I2">
-        <v>2</v>
+        <v>1465</v>
       </c>
       <c r="J2">
-        <v>0</v>
+        <v>1401</v>
       </c>
       <c r="K2">
-        <v>21</v>
+        <v>64</v>
       </c>
       <c r="L2">
-        <v>4</v>
+        <v>336</v>
+      </c>
+      <c r="M2">
+        <v>18</v>
       </c>
     </row>
     <row r="3">
@@ -478,16 +481,16 @@
         </is>
       </c>
       <c r="C3">
-        <v>138</v>
+        <v>15745</v>
       </c>
       <c r="D3">
-        <v>138</v>
+        <v>14938</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>807</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -496,19 +499,19 @@
         <v>0</v>
       </c>
       <c r="I3">
-        <v>18</v>
+        <v>2769</v>
       </c>
       <c r="J3">
-        <v>22</v>
+        <v>2670</v>
       </c>
       <c r="K3">
-        <v>49</v>
+        <v>5160</v>
       </c>
       <c r="L3">
-        <v>49</v>
+        <v>5146</v>
       </c>
       <c r="M3">
-        <v>22</v>
+        <v>10828</v>
       </c>
     </row>
     <row r="4">
@@ -523,16 +526,16 @@
         </is>
       </c>
       <c r="C4">
-        <v>66</v>
+        <v>10964</v>
       </c>
       <c r="D4">
-        <v>66</v>
+        <v>7039</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>3925</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -541,16 +544,19 @@
         <v>0</v>
       </c>
       <c r="I4">
-        <v>3</v>
+        <v>1015</v>
       </c>
       <c r="J4">
-        <v>4</v>
+        <v>736</v>
       </c>
       <c r="K4">
-        <v>44</v>
+        <v>5946</v>
       </c>
       <c r="L4">
-        <v>15</v>
+        <v>3267</v>
+      </c>
+      <c r="M4">
+        <v>723</v>
       </c>
     </row>
     <row r="5">
@@ -561,14 +567,14 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Integration</t>
+          <t>Humanitarian Transportation</t>
         </is>
       </c>
       <c r="C5">
-        <v>15</v>
+        <v>318</v>
       </c>
       <c r="D5">
-        <v>15</v>
+        <v>318</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -583,16 +589,16 @@
         <v>0</v>
       </c>
       <c r="I5">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="J5">
-        <v>0</v>
+        <v>66</v>
       </c>
       <c r="K5">
-        <v>13</v>
+        <v>123</v>
       </c>
       <c r="L5">
-        <v>2</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6">
@@ -603,20 +609,20 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Multipurpose CBI</t>
+          <t>Integration</t>
         </is>
       </c>
       <c r="C6">
-        <v>93</v>
+        <v>1767</v>
       </c>
       <c r="D6">
-        <v>93</v>
+        <v>1258</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>509</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -625,19 +631,19 @@
         <v>0</v>
       </c>
       <c r="I6">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="J6">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="K6">
-        <v>44</v>
+        <v>1232</v>
       </c>
       <c r="L6">
-        <v>20</v>
+        <v>535</v>
       </c>
       <c r="M6">
-        <v>93</v>
+        <v>519</v>
       </c>
     </row>
     <row r="7">
@@ -648,20 +654,20 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Protection (General)</t>
+          <t>Multipurpose CBI</t>
         </is>
       </c>
       <c r="C7">
-        <v>462</v>
+        <v>11275</v>
       </c>
       <c r="D7">
-        <v>451</v>
+        <v>10736</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
       <c r="F7">
-        <v>11</v>
+        <v>539</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -670,16 +676,19 @@
         <v>0</v>
       </c>
       <c r="I7">
-        <v>0</v>
+        <v>2584</v>
       </c>
       <c r="J7">
-        <v>0</v>
+        <v>2583</v>
       </c>
       <c r="K7">
-        <v>275</v>
+        <v>4001</v>
       </c>
       <c r="L7">
-        <v>187</v>
+        <v>2107</v>
+      </c>
+      <c r="M7">
+        <v>11275</v>
       </c>
     </row>
     <row r="8">
@@ -690,14 +699,14 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Shelter</t>
+          <t>Nutrition</t>
         </is>
       </c>
       <c r="C8">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D8">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -712,19 +721,16 @@
         <v>0</v>
       </c>
       <c r="I8">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J8">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K8">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="L8">
-        <v>5</v>
-      </c>
-      <c r="M8">
-        <v>17</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9">
@@ -735,20 +741,20 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>WASH</t>
+          <t>Protection (Child Protection)</t>
         </is>
       </c>
       <c r="C9">
-        <v>19</v>
+        <v>3708</v>
       </c>
       <c r="D9">
-        <v>19</v>
+        <v>3658</v>
       </c>
       <c r="E9">
         <v>0</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -757,16 +763,16 @@
         <v>0</v>
       </c>
       <c r="I9">
-        <v>5</v>
+        <v>2090</v>
       </c>
       <c r="J9">
-        <v>6</v>
+        <v>1911</v>
       </c>
       <c r="K9">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="L9">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -777,20 +783,20 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>Protection (GBV)</t>
         </is>
       </c>
       <c r="C10">
-        <v>838</v>
+        <v>0</v>
       </c>
       <c r="D10">
-        <v>827</v>
+        <v>0</v>
       </c>
       <c r="E10">
         <v>0</v>
       </c>
       <c r="F10">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="G10">
         <v>0</v>
@@ -799,34 +805,34 @@
         <v>0</v>
       </c>
       <c r="I10">
-        <v>52</v>
+        <v>0</v>
       </c>
       <c r="J10">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="K10">
-        <v>455</v>
+        <v>0</v>
       </c>
       <c r="L10">
-        <v>286</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>February</t>
+          <t>January</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Education</t>
+          <t>Protection (General)</t>
         </is>
       </c>
       <c r="C11">
-        <v>44</v>
+        <v>19907</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>19907</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -841,40 +847,43 @@
         <v>0</v>
       </c>
       <c r="I11">
-        <v>0</v>
+        <v>2096</v>
       </c>
       <c r="J11">
-        <v>0</v>
+        <v>2090</v>
       </c>
       <c r="K11">
-        <v>35</v>
+        <v>10063</v>
       </c>
       <c r="L11">
-        <v>9</v>
+        <v>5658</v>
+      </c>
+      <c r="M11">
+        <v>280</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>February</t>
+          <t>January</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Food Security</t>
+          <t>Shelter</t>
         </is>
       </c>
       <c r="C12">
-        <v>67</v>
+        <v>8178</v>
       </c>
       <c r="D12">
-        <v>67</v>
+        <v>8148</v>
       </c>
       <c r="E12">
         <v>0</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="G12">
         <v>0</v>
@@ -883,43 +892,43 @@
         <v>0</v>
       </c>
       <c r="I12">
-        <v>9</v>
+        <v>1472</v>
       </c>
       <c r="J12">
-        <v>7</v>
+        <v>1479</v>
       </c>
       <c r="K12">
-        <v>31</v>
+        <v>2348</v>
       </c>
       <c r="L12">
-        <v>20</v>
+        <v>2879</v>
       </c>
       <c r="M12">
-        <v>25</v>
+        <v>147</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>February</t>
+          <t>January</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Health</t>
+          <t>WASH</t>
         </is>
       </c>
       <c r="C13">
-        <v>771</v>
+        <v>4551</v>
       </c>
       <c r="D13">
-        <v>66</v>
+        <v>4447</v>
       </c>
       <c r="E13">
         <v>0</v>
       </c>
       <c r="F13">
-        <v>0</v>
+        <v>104</v>
       </c>
       <c r="G13">
         <v>0</v>
@@ -928,40 +937,43 @@
         <v>0</v>
       </c>
       <c r="I13">
-        <v>1</v>
+        <v>487</v>
       </c>
       <c r="J13">
-        <v>3</v>
+        <v>486</v>
       </c>
       <c r="K13">
-        <v>456</v>
+        <v>1608</v>
       </c>
       <c r="L13">
-        <v>311</v>
+        <v>1970</v>
+      </c>
+      <c r="M13">
+        <v>295</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>February</t>
+          <t>January</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Integration</t>
+          <t>All</t>
         </is>
       </c>
       <c r="C14">
-        <v>56</v>
+        <v>79982</v>
       </c>
       <c r="D14">
-        <v>32</v>
+        <v>73236</v>
       </c>
       <c r="E14">
         <v>0</v>
       </c>
       <c r="F14">
-        <v>0</v>
+        <v>6453</v>
       </c>
       <c r="G14">
         <v>0</v>
@@ -970,16 +982,16 @@
         <v>0</v>
       </c>
       <c r="I14">
-        <v>2</v>
+        <v>14009</v>
       </c>
       <c r="J14">
-        <v>6</v>
+        <v>13422</v>
       </c>
       <c r="K14">
-        <v>30</v>
+        <v>30545</v>
       </c>
       <c r="L14">
-        <v>18</v>
+        <v>22006</v>
       </c>
     </row>
     <row r="15">
@@ -990,20 +1002,20 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Multipurpose CBI</t>
+          <t>Education</t>
         </is>
       </c>
       <c r="C15">
-        <v>161</v>
+        <v>2289</v>
       </c>
       <c r="D15">
-        <v>161</v>
+        <v>2288</v>
       </c>
       <c r="E15">
         <v>0</v>
       </c>
       <c r="F15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G15">
         <v>0</v>
@@ -1012,19 +1024,16 @@
         <v>0</v>
       </c>
       <c r="I15">
-        <v>28</v>
+        <v>919</v>
       </c>
       <c r="J15">
-        <v>29</v>
+        <v>940</v>
       </c>
       <c r="K15">
-        <v>67</v>
+        <v>352</v>
       </c>
       <c r="L15">
-        <v>37</v>
-      </c>
-      <c r="M15">
-        <v>161</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16">
@@ -1035,20 +1044,20 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Protection (General)</t>
+          <t>Food Security</t>
         </is>
       </c>
       <c r="C16">
-        <v>504</v>
+        <v>16190</v>
       </c>
       <c r="D16">
-        <v>504</v>
+        <v>16051</v>
       </c>
       <c r="E16">
         <v>0</v>
       </c>
       <c r="F16">
-        <v>0</v>
+        <v>139</v>
       </c>
       <c r="G16">
         <v>0</v>
@@ -1057,16 +1066,19 @@
         <v>0</v>
       </c>
       <c r="I16">
-        <v>2</v>
+        <v>2887</v>
       </c>
       <c r="J16">
-        <v>2</v>
+        <v>3134</v>
       </c>
       <c r="K16">
-        <v>304</v>
+        <v>4925</v>
       </c>
       <c r="L16">
-        <v>196</v>
+        <v>5244</v>
+      </c>
+      <c r="M16">
+        <v>11979</v>
       </c>
     </row>
     <row r="17">
@@ -1077,20 +1089,20 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Shelter</t>
+          <t>Health</t>
         </is>
       </c>
       <c r="C17">
-        <v>16</v>
+        <v>10057</v>
       </c>
       <c r="D17">
-        <v>16</v>
+        <v>8358</v>
       </c>
       <c r="E17">
         <v>0</v>
       </c>
       <c r="F17">
-        <v>0</v>
+        <v>1699</v>
       </c>
       <c r="G17">
         <v>0</v>
@@ -1099,16 +1111,19 @@
         <v>0</v>
       </c>
       <c r="I17">
-        <v>4</v>
+        <v>975</v>
       </c>
       <c r="J17">
-        <v>4</v>
+        <v>879</v>
       </c>
       <c r="K17">
-        <v>4</v>
+        <v>5110</v>
       </c>
       <c r="L17">
-        <v>4</v>
+        <v>3055</v>
+      </c>
+      <c r="M17">
+        <v>1063</v>
       </c>
     </row>
     <row r="18">
@@ -1119,14 +1134,14 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>WASH</t>
+          <t>Humanitarian Transportation</t>
         </is>
       </c>
       <c r="C18">
-        <v>17</v>
+        <v>463</v>
       </c>
       <c r="D18">
-        <v>17</v>
+        <v>463</v>
       </c>
       <c r="E18">
         <v>0</v>
@@ -1141,16 +1156,19 @@
         <v>0</v>
       </c>
       <c r="I18">
-        <v>4</v>
+        <v>82</v>
       </c>
       <c r="J18">
+        <v>81</v>
+      </c>
+      <c r="K18">
+        <v>178</v>
+      </c>
+      <c r="L18">
+        <v>122</v>
+      </c>
+      <c r="M18">
         <v>5</v>
-      </c>
-      <c r="K18">
-        <v>4</v>
-      </c>
-      <c r="L18">
-        <v>4</v>
       </c>
     </row>
     <row r="19">
@@ -1161,20 +1179,20 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>Integration</t>
         </is>
       </c>
       <c r="C19">
-        <v>1636</v>
+        <v>1724</v>
       </c>
       <c r="D19">
-        <v>864</v>
+        <v>1566</v>
       </c>
       <c r="E19">
         <v>0</v>
       </c>
       <c r="F19">
-        <v>0</v>
+        <v>158</v>
       </c>
       <c r="G19">
         <v>0</v>
@@ -1183,40 +1201,43 @@
         <v>0</v>
       </c>
       <c r="I19">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="J19">
-        <v>56</v>
+        <v>0</v>
       </c>
       <c r="K19">
-        <v>931</v>
+        <v>1098</v>
       </c>
       <c r="L19">
-        <v>599</v>
+        <v>626</v>
+      </c>
+      <c r="M19">
+        <v>958</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>March</t>
+          <t>February</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Education</t>
+          <t>Multipurpose CBI</t>
         </is>
       </c>
       <c r="C20">
-        <v>55</v>
+        <v>11749</v>
       </c>
       <c r="D20">
-        <v>55</v>
+        <v>11497</v>
       </c>
       <c r="E20">
         <v>0</v>
       </c>
       <c r="F20">
-        <v>0</v>
+        <v>252</v>
       </c>
       <c r="G20">
         <v>0</v>
@@ -1225,40 +1246,43 @@
         <v>0</v>
       </c>
       <c r="I20">
-        <v>1</v>
+        <v>2694</v>
       </c>
       <c r="J20">
-        <v>0</v>
+        <v>2839</v>
       </c>
       <c r="K20">
-        <v>44</v>
+        <v>4110</v>
       </c>
       <c r="L20">
-        <v>10</v>
+        <v>2106</v>
+      </c>
+      <c r="M20">
+        <v>11749</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>March</t>
+          <t>February</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Food Security</t>
+          <t>Nutrition</t>
         </is>
       </c>
       <c r="C21">
-        <v>118</v>
+        <v>10</v>
       </c>
       <c r="D21">
-        <v>118</v>
+        <v>3</v>
       </c>
       <c r="E21">
         <v>0</v>
       </c>
       <c r="F21">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G21">
         <v>0</v>
@@ -1267,43 +1291,40 @@
         <v>0</v>
       </c>
       <c r="I21">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="J21">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="K21">
-        <v>43</v>
+        <v>10</v>
       </c>
       <c r="L21">
-        <v>37</v>
-      </c>
-      <c r="M21">
-        <v>71</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>March</t>
+          <t>February</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Health</t>
+          <t>Protection (Child Protection)</t>
         </is>
       </c>
       <c r="C22">
-        <v>59</v>
+        <v>2915</v>
       </c>
       <c r="D22">
-        <v>59</v>
+        <v>2785</v>
       </c>
       <c r="E22">
         <v>0</v>
       </c>
       <c r="F22">
-        <v>0</v>
+        <v>130</v>
       </c>
       <c r="G22">
         <v>0</v>
@@ -1312,34 +1333,34 @@
         <v>0</v>
       </c>
       <c r="I22">
-        <v>3</v>
+        <v>1679</v>
       </c>
       <c r="J22">
-        <v>0</v>
+        <v>1552</v>
       </c>
       <c r="K22">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="L22">
-        <v>22</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>March</t>
+          <t>February</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Integration</t>
+          <t>Protection (GBV)</t>
         </is>
       </c>
       <c r="C23">
-        <v>48</v>
+        <v>0</v>
       </c>
       <c r="D23">
-        <v>48</v>
+        <v>0</v>
       </c>
       <c r="E23">
         <v>0</v>
@@ -1360,28 +1381,28 @@
         <v>0</v>
       </c>
       <c r="K23">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="L23">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>March</t>
+          <t>February</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Multipurpose CBI</t>
+          <t>Protection (General)</t>
         </is>
       </c>
       <c r="C24">
-        <v>124</v>
+        <v>18530</v>
       </c>
       <c r="D24">
-        <v>124</v>
+        <v>18530</v>
       </c>
       <c r="E24">
         <v>0</v>
@@ -1396,37 +1417,37 @@
         <v>0</v>
       </c>
       <c r="I24">
-        <v>10</v>
+        <v>1934</v>
       </c>
       <c r="J24">
-        <v>33</v>
+        <v>1861</v>
       </c>
       <c r="K24">
-        <v>44</v>
+        <v>9276</v>
       </c>
       <c r="L24">
-        <v>37</v>
+        <v>5391</v>
       </c>
       <c r="M24">
-        <v>124</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>March</t>
+          <t>February</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Protection (GBV)</t>
+          <t>Protection (Human Trafficking &amp; Smuggling)</t>
         </is>
       </c>
       <c r="C25">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D25">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E25">
         <v>0</v>
@@ -1447,7 +1468,7 @@
         <v>0</v>
       </c>
       <c r="K25">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L25">
         <v>0</v>
@@ -1456,25 +1477,25 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>March</t>
+          <t>February</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Protection (General)</t>
+          <t>Shelter</t>
         </is>
       </c>
       <c r="C26">
-        <v>299</v>
+        <v>7608</v>
       </c>
       <c r="D26">
-        <v>299</v>
+        <v>7583</v>
       </c>
       <c r="E26">
         <v>0</v>
       </c>
       <c r="F26">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="G26">
         <v>0</v>
@@ -1483,43 +1504,43 @@
         <v>0</v>
       </c>
       <c r="I26">
-        <v>2</v>
+        <v>1512</v>
       </c>
       <c r="J26">
-        <v>1</v>
+        <v>1659</v>
       </c>
       <c r="K26">
-        <v>186</v>
+        <v>2154</v>
       </c>
       <c r="L26">
-        <v>110</v>
+        <v>2281</v>
       </c>
       <c r="M26">
-        <v>7</v>
+        <v>419</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>March</t>
+          <t>February</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Shelter</t>
+          <t>WASH</t>
         </is>
       </c>
       <c r="C27">
-        <v>8</v>
+        <v>5677</v>
       </c>
       <c r="D27">
-        <v>8</v>
+        <v>5598</v>
       </c>
       <c r="E27">
         <v>0</v>
       </c>
       <c r="F27">
-        <v>0</v>
+        <v>79</v>
       </c>
       <c r="G27">
         <v>0</v>
@@ -1528,40 +1549,43 @@
         <v>0</v>
       </c>
       <c r="I27">
-        <v>0</v>
+        <v>547</v>
       </c>
       <c r="J27">
-        <v>0</v>
+        <v>578</v>
       </c>
       <c r="K27">
-        <v>2</v>
+        <v>2050</v>
       </c>
       <c r="L27">
-        <v>6</v>
+        <v>2502</v>
+      </c>
+      <c r="M27">
+        <v>907</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>March</t>
+          <t>February</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>WASH</t>
+          <t>All</t>
         </is>
       </c>
       <c r="C28">
-        <v>50</v>
+        <v>77425</v>
       </c>
       <c r="D28">
-        <v>50</v>
+        <v>74728</v>
       </c>
       <c r="E28">
         <v>0</v>
       </c>
       <c r="F28">
-        <v>0</v>
+        <v>2490</v>
       </c>
       <c r="G28">
         <v>0</v>
@@ -1570,16 +1594,16 @@
         <v>0</v>
       </c>
       <c r="I28">
-        <v>11</v>
+        <v>13229</v>
       </c>
       <c r="J28">
-        <v>13</v>
+        <v>13523</v>
       </c>
       <c r="K28">
-        <v>13</v>
+        <v>29268</v>
       </c>
       <c r="L28">
-        <v>13</v>
+        <v>21405</v>
       </c>
     </row>
     <row r="29">
@@ -1590,38 +1614,512 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
+          <t>Education</t>
+        </is>
+      </c>
+      <c r="C29">
+        <v>306</v>
+      </c>
+      <c r="D29">
+        <v>161</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>145</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <v>154</v>
+      </c>
+      <c r="J29">
+        <v>151</v>
+      </c>
+      <c r="K29">
+        <v>1</v>
+      </c>
+      <c r="L29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>March</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Food Security</t>
+        </is>
+      </c>
+      <c r="C30">
+        <v>12752</v>
+      </c>
+      <c r="D30">
+        <v>12698</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>54</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <v>2658</v>
+      </c>
+      <c r="J30">
+        <v>2632</v>
+      </c>
+      <c r="K30">
+        <v>3864</v>
+      </c>
+      <c r="L30">
+        <v>3598</v>
+      </c>
+      <c r="M30">
+        <v>12652</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>March</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Health</t>
+        </is>
+      </c>
+      <c r="C31">
+        <v>586</v>
+      </c>
+      <c r="D31">
+        <v>495</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>91</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <v>20</v>
+      </c>
+      <c r="J31">
+        <v>25</v>
+      </c>
+      <c r="K31">
+        <v>470</v>
+      </c>
+      <c r="L31">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>March</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Integration</t>
+        </is>
+      </c>
+      <c r="C32">
+        <v>1690</v>
+      </c>
+      <c r="D32">
+        <v>1447</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <v>243</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="I32">
+        <v>0</v>
+      </c>
+      <c r="J32">
+        <v>0</v>
+      </c>
+      <c r="K32">
+        <v>1246</v>
+      </c>
+      <c r="L32">
+        <v>444</v>
+      </c>
+      <c r="M32">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>March</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Multipurpose CBI</t>
+        </is>
+      </c>
+      <c r="C33">
+        <v>9769</v>
+      </c>
+      <c r="D33">
+        <v>9769</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
+      <c r="I33">
+        <v>2576</v>
+      </c>
+      <c r="J33">
+        <v>2502</v>
+      </c>
+      <c r="K33">
+        <v>3024</v>
+      </c>
+      <c r="L33">
+        <v>1667</v>
+      </c>
+      <c r="M33">
+        <v>9769</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>March</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Protection (Child Protection)</t>
+        </is>
+      </c>
+      <c r="C34">
+        <v>3718</v>
+      </c>
+      <c r="D34">
+        <v>3357</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <v>361</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
+      <c r="H34">
+        <v>0</v>
+      </c>
+      <c r="I34">
+        <v>1946</v>
+      </c>
+      <c r="J34">
+        <v>1772</v>
+      </c>
+      <c r="K34">
+        <v>0</v>
+      </c>
+      <c r="L34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>March</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Protection (GBV)</t>
+        </is>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+      <c r="I35">
+        <v>0</v>
+      </c>
+      <c r="J35">
+        <v>0</v>
+      </c>
+      <c r="K35">
+        <v>0</v>
+      </c>
+      <c r="L35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>March</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Protection (General)</t>
+        </is>
+      </c>
+      <c r="C36">
+        <v>16524</v>
+      </c>
+      <c r="D36">
+        <v>16524</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
+      <c r="G36">
+        <v>0</v>
+      </c>
+      <c r="H36">
+        <v>0</v>
+      </c>
+      <c r="I36">
+        <v>2336</v>
+      </c>
+      <c r="J36">
+        <v>2309</v>
+      </c>
+      <c r="K36">
+        <v>7656</v>
+      </c>
+      <c r="L36">
+        <v>4223</v>
+      </c>
+      <c r="M36">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>March</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Protection (Human Trafficking &amp; Smuggling)</t>
+        </is>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="F37">
+        <v>0</v>
+      </c>
+      <c r="G37">
+        <v>0</v>
+      </c>
+      <c r="H37">
+        <v>0</v>
+      </c>
+      <c r="I37">
+        <v>0</v>
+      </c>
+      <c r="J37">
+        <v>0</v>
+      </c>
+      <c r="K37">
+        <v>1</v>
+      </c>
+      <c r="L37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>March</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Shelter</t>
+        </is>
+      </c>
+      <c r="C38">
+        <v>3671</v>
+      </c>
+      <c r="D38">
+        <v>3670</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+      <c r="F38">
+        <v>1</v>
+      </c>
+      <c r="G38">
+        <v>0</v>
+      </c>
+      <c r="H38">
+        <v>0</v>
+      </c>
+      <c r="I38">
+        <v>1569</v>
+      </c>
+      <c r="J38">
+        <v>1568</v>
+      </c>
+      <c r="K38">
+        <v>277</v>
+      </c>
+      <c r="L38">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>March</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>WASH</t>
+        </is>
+      </c>
+      <c r="C39">
+        <v>1037</v>
+      </c>
+      <c r="D39">
+        <v>1037</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+      <c r="G39">
+        <v>0</v>
+      </c>
+      <c r="H39">
+        <v>0</v>
+      </c>
+      <c r="I39">
+        <v>10</v>
+      </c>
+      <c r="J39">
+        <v>7</v>
+      </c>
+      <c r="K39">
+        <v>510</v>
+      </c>
+      <c r="L39">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>March</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
           <t>All</t>
         </is>
       </c>
-      <c r="C29">
-        <v>765</v>
-      </c>
-      <c r="D29">
-        <v>765</v>
-      </c>
-      <c r="E29">
-        <v>0</v>
-      </c>
-      <c r="F29">
-        <v>0</v>
-      </c>
-      <c r="G29">
-        <v>0</v>
-      </c>
-      <c r="H29">
-        <v>0</v>
-      </c>
-      <c r="I29">
-        <v>49</v>
-      </c>
-      <c r="J29">
-        <v>63</v>
-      </c>
-      <c r="K29">
-        <v>402</v>
-      </c>
-      <c r="L29">
-        <v>251</v>
+      <c r="C40">
+        <v>50054</v>
+      </c>
+      <c r="D40">
+        <v>49159</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="F40">
+        <v>895</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
+      </c>
+      <c r="H40">
+        <v>0</v>
+      </c>
+      <c r="I40">
+        <v>11269</v>
+      </c>
+      <c r="J40">
+        <v>10966</v>
+      </c>
+      <c r="K40">
+        <v>17049</v>
+      </c>
+      <c r="L40">
+        <v>10770</v>
       </c>
     </row>
   </sheetData>

</xml_diff>